<commit_message>
modification au fichierIsa, FichierDangereux et fichierPascal
</commit_message>
<xml_diff>
--- a/FichierDangereux.xlsx
+++ b/FichierDangereux.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FF0CF4F6-A18F-4CA7-B80F-2373F0D0F2D3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FD9F28F0-4E57-4733-A3A8-FF30543B360C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,9 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Ne pas ouvrir sinon c'est la mort</t>
+  </si>
+  <si>
+    <t>même pas vrai!!!</t>
+  </si>
+  <si>
+    <t>;)</t>
   </si>
 </sst>
 </file>
@@ -340,15 +346,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>